<commit_message>
update data, complete notebook
</commit_message>
<xml_diff>
--- a/data/raw/starwars_messy.xlsx
+++ b/data/raw/starwars_messy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/GitHub/DSS/research-02/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3479EAA4-A5BC-F14A-A689-F2A2D22247A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CAD5E8-508A-6E40-9367-286AC7969C5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="440" windowWidth="14400" windowHeight="17560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1602,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C99F5C9-813F-AF46-AA73-0287A75AA01F}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:J95"/>
     </sheetView>
   </sheetViews>
@@ -7342,7 +7342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295129D2-91A9-5547-BC0E-6EDF02CA54E8}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>

</xml_diff>